<commit_message>
remove all sleep in ongoing message
</commit_message>
<xml_diff>
--- a/testcase.xlsx
+++ b/testcase.xlsx
@@ -12,10 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175"/>
   </bookViews>
   <sheets>
-    <sheet name="testcase_testcasetype" sheetId="1" r:id="rId1"/>
+    <sheet name="testcase" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">testcase_testcasetype!$A$1:$K$299</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">testcase!$A$1:$K$299</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -4039,7 +4039,7 @@
   <dimension ref="A1:K299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>